<commit_message>
Fix: Corrected patient avatar filenames
</commit_message>
<xml_diff>
--- a/patients.xlsx
+++ b/patients.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jespernillius/Desktop/My-project/game-backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89A841C0-48BE-404F-B3E0-BAA4ADEDD535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53DCD4A9-2026-E346-A76D-E381B67725F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -176,9 +176,6 @@
     <t>patient_avatar</t>
   </si>
   <si>
-    <t>britta.png</t>
-  </si>
-  <si>
     <t>Sten</t>
   </si>
   <si>
@@ -218,9 +215,6 @@
 När läkaren frågar "Vad för dig hit idag?", börja med det mest akuta (urinen och utslagen) men försök sedan att backa bandet och berätta hela historien. Var ärlig med din oro och din trötthet. Använd dina egna ord, som "känns som jag har grus i maskineriet" eller "orken är helt borta". Du är en vanlig person som drabbats av något du absolut inte förstår.</t>
   </si>
   <si>
-    <t>bengt.png</t>
-  </si>
-  <si>
     <t>allRadiologyTests</t>
   </si>
   <si>
@@ -374,9 +368,6 @@
     <t>ECG-Atrial-Fibrillation.jpg</t>
   </si>
   <si>
-    <t>frank.png</t>
-  </si>
-  <si>
     <t>["Hjärta", "Lungor", "Buk", "ekg", "seloken", "tiamin"]</t>
   </si>
   <si>
@@ -417,6 +408,9 @@
   </si>
   <si>
     <t>TRUE</t>
+  </si>
+  <si>
+    <t>Hubert.png</t>
   </si>
   <si>
     <t>Buksmärta</t>
@@ -483,9 +477,6 @@
   <si>
     <t>Du heter Hubert, är 55 år gammal och träffar nu en läkare på akutmottagningen. Du har sökt eftersom du 12 timmar tillbaka haft kontinuerlig smärta under höger revbensbåge, med utstrålning till höger i ryggen. (men detta uttrycker du givetvis som en patient hade gjort det). 
 Du har ont vid rörelse och djup inandning. Du medicinerar för högt blodtryck med Losartan och har tidigare varit behandlad med SSRI för en depression för 10 år sedan. Du är lite febrig sedan några timmar tillbaka. Du har tog en alvedon på 1 g för 1 timme sedan, har inte märkt påtaglig effekt på smärtan. Febrig känner du dig fortfarande. Du har inga problem med andningen. Du är lite överviktig, och äter mycket vetelängder. Du tycker smärtan är 8/10, och är molande. Du är adopterad och har inga levande släktingar, så du vet inte om din hereditet. Du bor i en lägenhet själv och jobbar med statsförvaltning på hög nivå. Du tränar någon gång i veckan. Du röker sällan, bara på fest. Du dricker vin ibland kanske 1 gång i veckan, något enstaka glas. Du är inte allergisk mot några mediciner eller så. Du har en gång tidigare haft väldigt ont på samma ställe, men det gick över och du sökta aldrig för det.</t>
-  </si>
-  <si>
-    <t>hubert.png</t>
   </si>
   <si>
     <t>Adipös. Kraftigt palpationsöm över höger arcus med defence. Mjuk buk. Viss diffus ömhet i hela buken. Ej dunköm över njurlogerna. Muphey's sign negativt.</t>
@@ -613,6 +604,15 @@
   </si>
   <si>
     <t>["blododling", "evf", "ld", "urinodling", "ringer"]</t>
+  </si>
+  <si>
+    <t>Britta.png</t>
+  </si>
+  <si>
+    <t>Bengt.png</t>
+  </si>
+  <si>
+    <t>Frank.png</t>
   </si>
 </sst>
 </file>
@@ -988,8 +988,8 @@
   <dimension ref="A1:DP8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="DH1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DL12" sqref="DL12"/>
+      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1118,7 +1118,7 @@
       <c r="CY1" s="11"/>
       <c r="CZ1" s="11"/>
       <c r="DA1" s="12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="DB1" s="12"/>
       <c r="DC1" s="12"/>
@@ -1138,13 +1138,13 @@
         <v>37</v>
       </c>
       <c r="DN1" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="DO1" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="DP1" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:120" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1155,7 +1155,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>9</v>
@@ -1164,16 +1164,16 @@
         <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>46</v>
@@ -1233,109 +1233,109 @@
         <v>33</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="AD2" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="AE2" s="1"/>
       <c r="AF2" s="1"/>
       <c r="AG2" s="1"/>
       <c r="AI2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AK2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="AJ2" s="1" t="s">
+      <c r="AL2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="AK2" s="1" t="s">
+      <c r="AM2" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="AL2" s="1" t="s">
+      <c r="AN2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="AM2" s="1" t="s">
+      <c r="AO2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AN2" s="1" t="s">
+      <c r="AP2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="AO2" s="1" t="s">
+      <c r="AQ2" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="AP2" s="1" t="s">
+      <c r="AR2" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AQ2" s="1" t="s">
+      <c r="AS2" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="AT2" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="AR2" s="1" t="s">
+      <c r="AU2" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="AS2" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="AT2" s="1" t="s">
+      <c r="AV2" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="AU2" s="1" t="s">
+      <c r="AW2" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="AV2" s="1" t="s">
+      <c r="AX2" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AW2" s="1" t="s">
+      <c r="AY2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AX2" s="1" t="s">
+      <c r="AZ2" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AY2" s="1" t="s">
+      <c r="BA2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AZ2" s="1" t="s">
+      <c r="BB2" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="BA2" s="1" t="s">
+      <c r="BC2" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="BB2" s="1" t="s">
+      <c r="BD2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="BC2" s="1" t="s">
+      <c r="BE2" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="BD2" s="1" t="s">
+      <c r="BF2" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="BE2" s="1" t="s">
+      <c r="BG2" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="BF2" s="1" t="s">
+      <c r="BH2" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="BG2" s="1" t="s">
+      <c r="BI2" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="BH2" s="1" t="s">
+      <c r="BJ2" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="BI2" s="1" t="s">
+      <c r="BK2" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="BJ2" s="1" t="s">
+      <c r="BL2" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="BK2" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="BL2" s="1" t="s">
-        <v>85</v>
-      </c>
       <c r="BM2" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="BN2" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="BN2" s="1" t="s">
-        <v>170</v>
       </c>
       <c r="BO2" s="1"/>
       <c r="BP2" s="1"/>
@@ -1380,25 +1380,25 @@
         <v>43</v>
       </c>
       <c r="CY2" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="CZ2" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="DA2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="DB2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="DC2" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="DB2" s="1" t="s">
+      <c r="DD2" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="DC2" s="1" t="s">
+      <c r="DE2" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="DD2" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="DE2" s="1" t="s">
-        <v>90</v>
       </c>
       <c r="DF2" s="1"/>
       <c r="DG2" s="1" t="s">
@@ -1411,25 +1411,25 @@
         <v>26</v>
       </c>
       <c r="DJ2" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="DK2" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="DL2" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="DM2" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="DN2" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="DO2" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="DP2" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="DK2" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="DL2" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="DM2" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="DN2" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="DO2" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="DP2" s="3" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="3" spans="1:120" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1440,20 +1440,20 @@
         <v>82</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>41</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="5" t="s">
-        <v>47</v>
+        <v>176</v>
       </c>
       <c r="K3" s="5">
         <v>26</v>
@@ -1532,44 +1532,44 @@
         <v>27</v>
       </c>
       <c r="DH3" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="DI3" s="1"/>
       <c r="DJ3" s="1" t="s">
         <v>30</v>
       </c>
       <c r="DL3" s="16" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="DM3" s="1" t="s">
         <v>38</v>
       </c>
       <c r="DP3" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:120" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4" s="1">
         <v>62</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
       <c r="H4" s="15"/>
       <c r="I4" s="15"/>
       <c r="J4" s="1" t="s">
-        <v>53</v>
+        <v>177</v>
       </c>
       <c r="K4" s="1">
         <v>20</v>
@@ -1593,7 +1593,7 @@
         <v>1</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
@@ -1603,14 +1603,14 @@
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
       <c r="AA4" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="AB4" s="1"/>
       <c r="AC4" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="AD4" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="AE4" s="1"/>
       <c r="AF4" s="1"/>
@@ -1640,13 +1640,13 @@
       </c>
       <c r="BM4" s="3"/>
       <c r="CV4" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="CW4" s="3"/>
       <c r="CX4" s="3"/>
       <c r="CY4" s="3"/>
       <c r="CZ4" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="DA4" s="3"/>
       <c r="DB4" s="3"/>
@@ -1657,44 +1657,44 @@
         <v>27</v>
       </c>
       <c r="DH4" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="DI4" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="DJ4" s="1"/>
       <c r="DL4" s="3" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="DM4" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="DP4" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:120" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B5" s="1">
         <v>75</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1" t="s">
-        <v>105</v>
+        <v>178</v>
       </c>
       <c r="K5" s="1">
         <v>24</v>
@@ -1718,13 +1718,13 @@
         <v>1</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="AC5" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="AO5">
         <v>136</v>
@@ -1736,10 +1736,10 @@
         <v>634</v>
       </c>
       <c r="CW5" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="CX5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="CY5" s="3"/>
       <c r="CZ5" s="3"/>
@@ -1747,55 +1747,55 @@
         <v>27</v>
       </c>
       <c r="DH5" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="DI5" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="DJ5" s="1" t="s">
         <v>34</v>
       </c>
       <c r="DK5" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="DL5" s="3" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="DM5" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="DN5" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="DO5" s="3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="DP5" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:120" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B6" s="3">
         <v>55</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
       <c r="H6" s="17"/>
       <c r="I6" s="17"/>
       <c r="J6" s="3" t="s">
-        <v>140</v>
+        <v>117</v>
       </c>
       <c r="K6" s="3">
         <v>18</v>
@@ -1821,7 +1821,7 @@
       <c r="R6" s="3"/>
       <c r="S6" s="3"/>
       <c r="T6" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="U6" s="3"/>
       <c r="V6" s="3"/>
@@ -1857,7 +1857,7 @@
       <c r="AV6" s="3"/>
       <c r="AW6" s="3"/>
       <c r="AX6" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="AY6" s="3"/>
       <c r="AZ6" s="3"/>
@@ -1916,7 +1916,7 @@
       <c r="DA6" s="3"/>
       <c r="DB6" s="3"/>
       <c r="DC6" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="DD6" s="3"/>
       <c r="DE6" s="3"/>
@@ -1925,55 +1925,55 @@
         <v>27</v>
       </c>
       <c r="DH6" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="DI6" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="DJ6" s="3"/>
       <c r="DK6" s="3"/>
       <c r="DL6" s="3" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="DM6" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="DN6" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="DO6" s="3"/>
       <c r="DP6" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:120" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B7" s="3">
         <v>4</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="K7" s="3">
         <v>23</v>
@@ -1999,26 +1999,26 @@
       <c r="R7" s="3"/>
       <c r="S7" s="3"/>
       <c r="T7" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="U7" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="V7" s="3" t="s">
         <v>126</v>
-      </c>
-      <c r="U7" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="V7" s="3" t="s">
-        <v>128</v>
       </c>
       <c r="W7" s="3"/>
       <c r="X7" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="Y7" s="3"/>
       <c r="Z7" s="3"/>
       <c r="AA7" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="AB7" s="3"/>
       <c r="AC7" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="AD7" s="3"/>
       <c r="AE7" s="3"/>
@@ -2103,7 +2103,7 @@
       <c r="CT7" s="3"/>
       <c r="CU7" s="3"/>
       <c r="CV7" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="CW7" s="3"/>
       <c r="CX7" s="3"/>
@@ -2119,47 +2119,47 @@
         <v>27</v>
       </c>
       <c r="DH7" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="DI7" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="DJ7" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="DK7" s="3"/>
       <c r="DL7" s="3" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="DM7" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="DN7" s="17" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="DO7" s="3"/>
       <c r="DP7" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:120" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B8" s="1">
         <v>44</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="K8">
         <v>16</v>
@@ -2183,16 +2183,16 @@
         <v>1</v>
       </c>
       <c r="T8" s="3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="V8" s="3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="AI8">
         <v>166</v>
       </c>
       <c r="AJ8" s="3" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="AM8">
         <v>170</v>
@@ -2222,28 +2222,28 @@
         <v>5</v>
       </c>
       <c r="CV8" s="3" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="CZ8" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="DG8" s="1" t="s">
         <v>27</v>
       </c>
       <c r="DH8" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="DI8" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="DK8" s="3" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="DL8" s="17" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="DM8" s="3" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Add case rating and feedback system
</commit_message>
<xml_diff>
--- a/patients.xlsx
+++ b/patients.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jespernillius/Desktop/My-project/game-backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53DCD4A9-2026-E346-A76D-E381B67725F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD3F919-B3A0-E945-AE84-849FF2AAD005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-9000" yWindow="2100" windowWidth="29400" windowHeight="18360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hmm, Im not sure that my google" sheetId="1" r:id="rId1"/>
@@ -597,9 +597,6 @@
     <t>Sorkfeber</t>
   </si>
   <si>
-    <t>patrik.png</t>
-  </si>
-  <si>
     <t>["Hjärta", "Lungor", "Buk", "Mun och Svalg", "Hud", "Underben", "hb", "lpk", "tpk", "crp", "na", "k", "krea", "urea", "asat", "alat", ["dt-njursten", "UL-njurar"], "pumulaserologi"]</t>
   </si>
   <si>
@@ -613,6 +610,9 @@
   </si>
   <si>
     <t>Frank.png</t>
+  </si>
+  <si>
+    <t>Patrik.png</t>
   </si>
 </sst>
 </file>
@@ -989,7 +989,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J12" sqref="J12"/>
+      <selection pane="topRight" activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1453,7 +1453,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K3" s="5">
         <v>26</v>
@@ -1569,7 +1569,7 @@
       <c r="H4" s="15"/>
       <c r="I4" s="15"/>
       <c r="J4" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K4" s="1">
         <v>20</v>
@@ -1694,7 +1694,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K5" s="1">
         <v>24</v>
@@ -2159,7 +2159,7 @@
         <v>166</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="K8">
         <v>16</v>
@@ -2231,10 +2231,10 @@
         <v>27</v>
       </c>
       <c r="DH8" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="DI8" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="DI8" s="1" t="s">
-        <v>175</v>
       </c>
       <c r="DK8" s="3" t="s">
         <v>170</v>

</xml_diff>